<commit_message>
Last Friday 1.07 update
</commit_message>
<xml_diff>
--- a/kernels.xlsx
+++ b/kernels.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="straw.avi" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Linear</t>
   </si>
@@ -58,12 +59,21 @@
   <si>
     <t>Sample</t>
   </si>
+  <si>
+    <t>attempt</t>
+  </si>
+  <si>
+    <t>Random initialization</t>
+  </si>
+  <si>
+    <t>Pseudo-random initialization</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +85,23 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -116,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -126,6 +153,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -183,7 +226,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -542,11 +584,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1345288224"/>
-        <c:axId val="1345287136"/>
+        <c:axId val="1024416672"/>
+        <c:axId val="1024408512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1345288224"/>
+        <c:axId val="1024416672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -589,7 +631,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1345287136"/>
+        <c:crossAx val="1024408512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -597,7 +639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1345287136"/>
+        <c:axId val="1024408512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,7 +690,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1345288224"/>
+        <c:crossAx val="1024416672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -662,6 +704,1001 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Kernel</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> weights</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>straw.avi!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>straw.avi!$B$4:$G$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>straw.avi!$E$4:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Poly</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RatQuad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>straw.avi!$B$5:$G$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>straw.avi!$E$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90815072719967405</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1849272800325704E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>straw.avi!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>straw.avi!$B$4:$G$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>straw.avi!$E$4:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Poly</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RatQuad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>straw.avi!$B$6:$G$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>straw.avi!$E$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.69694011455729E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71153252919704801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28577053068839497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>straw.avi!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>straw.avi!$B$4:$G$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>straw.avi!$E$4:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Poly</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RatQuad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>straw.avi!$B$7:$G$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>straw.avi!$E$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.5361061437881497E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.982082584994869</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3813088613422992E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>straw.avi!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>straw.avi!$B$4:$G$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>straw.avi!$E$4:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Poly</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RatQuad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>straw.avi!$B$8:$G$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>straw.avi!$E$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.3512555785249303E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89690992195308095</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8738822468394202E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1024406336"/>
+        <c:axId val="1024404160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1024406336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1024404160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1024404160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1024406336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Kernel weights</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>straw.avi!$E$19:$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Poly</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RatQuad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>straw.avi!$E$20:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.6905385714016806E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83007198613533395</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16123747529326399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>straw.avi!$E$19:$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Poly</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RatQuad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>straw.avi!$E$21:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.38847221277719E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99420848761949898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0304016772374301E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>straw.avi!$E$19:$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Poly</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RatQuad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>straw.avi!$E$22:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.6905385714016806E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83007198613533395</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16123747529326399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1182353264"/>
+        <c:axId val="1182355984"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1182353264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1182355984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1182355984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1182353264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -769,7 +1806,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1299,6 +3422,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1572,8 +3760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1698,4 +3886,262 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.90815072719967405</v>
+      </c>
+      <c r="G5" s="6">
+        <v>9.1849272800325704E-2</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2.69694011455729E-3</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.71153252919704801</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.28577053068839497</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>8.5361061437881497E-3</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.982082584994869</v>
+      </c>
+      <c r="G7" s="6">
+        <v>9.3813088613422992E-3</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="6">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>4.3512555785249303E-3</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.89690992195308095</v>
+      </c>
+      <c r="G8" s="7">
+        <v>9.8738822468394202E-2</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6">
+        <v>8.6905385714016806E-3</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.83007198613533395</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.16123747529326399</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="6">
+        <v>6</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <v>5.38847221277719E-3</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.99420848761949898</v>
+      </c>
+      <c r="G21" s="6">
+        <v>4.0304016772374301E-4</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="6">
+        <v>10</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
+        <v>8.6905385714016806E-3</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.83007198613533395</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0.16123747529326399</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="6"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>